<commit_message>
Fixed typo, changed contextual parameters to use container OID constants from APDUConstants.java
</commit_message>
<xml_diff>
--- a/docs/85b_test_definitions_PIV_Production.xlsx
+++ b/docs/85b_test_definitions_PIV_Production.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bob.fontana\Documents\GitRepos\piv-conformance\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{27A00063-9522-4DAB-949A-BDE62FDCDE2A}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D56A504C-51FF-491B-BFCC-891CA29E9606}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5700" yWindow="780" windowWidth="23040" windowHeight="12120" tabRatio="634" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="5700" yWindow="780" windowWidth="23040" windowHeight="12120" tabRatio="634" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PIV I Reference Tests" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1200" uniqueCount="786">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1197" uniqueCount="785">
   <si>
     <t>Test Case</t>
   </si>
@@ -2358,12 +2358,6 @@
     <t>Validate that facial image CBEFF FASC-N field contains the same 25 bytes as the FASC-N component of the CHUID identifier</t>
   </si>
   <si>
-    <t>Cardholder Fingerprints==513,Cardholder Facial Image==1281</t>
-  </si>
-  <si>
-    <t>Cardholder Fingerprints==224,Cardholder Facial Image==32</t>
-  </si>
-  <si>
     <t>Verify that the CBEFF Biometric Data Block (BDB) Format Type is set to the appropriate value</t>
   </si>
   <si>
@@ -2385,10 +2379,13 @@
     <t>Verify that FASC-N field in the CBEFF FASC-N contains the same 25 bytes as the FASC-N component of the CHUID identifier</t>
   </si>
   <si>
-    <t>You might want to change this parameter format</t>
-  </si>
-  <si>
-    <t>Cardholder Fingerprints==8,Cardholder Facial Image==2</t>
+    <t>CARDHOLDER_FINGERPRINTS_OID:513,CARDHOLDER_FACIAL_IMAGE_OID:1281</t>
+  </si>
+  <si>
+    <t>CARDHOLDER_FINGERPRINTS_OID:8,CARDHOLDER_FACIAL_IMAGE_OID:2</t>
+  </si>
+  <si>
+    <t>CARDHOLDER_FINGERPRINTS_OID,224:CARDHOLDER_FACIAL_IMAGE_OID:32</t>
   </si>
 </sst>
 </file>
@@ -2449,7 +2446,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -2470,11 +2467,6 @@
       <alignment vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
@@ -2868,7 +2860,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E209"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="G109" sqref="G109"/>
     </sheetView>
   </sheetViews>
@@ -3629,7 +3621,7 @@
       <c r="A86" s="9" t="s">
         <v>716</v>
       </c>
-      <c r="B86" s="10" t="s">
+      <c r="B86" s="9" t="s">
         <v>689</v>
       </c>
       <c r="C86" s="8" t="s">
@@ -3640,10 +3632,10 @@
       <c r="A87" s="9" t="s">
         <v>720</v>
       </c>
-      <c r="B87" s="10" t="s">
+      <c r="B87" s="9" t="s">
         <v>699</v>
       </c>
-      <c r="C87" s="10" t="s">
+      <c r="C87" s="9" t="s">
         <v>575</v>
       </c>
     </row>
@@ -3651,7 +3643,7 @@
       <c r="A88" s="9" t="s">
         <v>721</v>
       </c>
-      <c r="B88" s="10" t="s">
+      <c r="B88" s="9" t="s">
         <v>690</v>
       </c>
       <c r="C88" s="8" t="s">
@@ -3662,7 +3654,7 @@
       <c r="A89" s="9" t="s">
         <v>722</v>
       </c>
-      <c r="B89" s="10" t="s">
+      <c r="B89" s="9" t="s">
         <v>700</v>
       </c>
       <c r="C89" s="8" t="s">
@@ -3673,7 +3665,7 @@
       <c r="A90" s="9" t="s">
         <v>723</v>
       </c>
-      <c r="B90" s="10" t="s">
+      <c r="B90" s="9" t="s">
         <v>702</v>
       </c>
       <c r="C90" s="8" t="s">
@@ -3684,7 +3676,7 @@
       <c r="A91" s="9" t="s">
         <v>724</v>
       </c>
-      <c r="B91" s="10" t="s">
+      <c r="B91" s="9" t="s">
         <v>701</v>
       </c>
       <c r="C91" s="8" t="s">
@@ -3695,7 +3687,7 @@
       <c r="A92" s="9" t="s">
         <v>725</v>
       </c>
-      <c r="B92" s="10" t="s">
+      <c r="B92" s="9" t="s">
         <v>696</v>
       </c>
       <c r="C92" s="8" t="s">
@@ -3706,10 +3698,10 @@
       <c r="A93" s="9" t="s">
         <v>726</v>
       </c>
-      <c r="B93" s="10" t="s">
+      <c r="B93" s="9" t="s">
         <v>714</v>
       </c>
-      <c r="C93" s="10" t="s">
+      <c r="C93" s="9" t="s">
         <v>715</v>
       </c>
     </row>
@@ -3717,10 +3709,10 @@
       <c r="A94" s="9" t="s">
         <v>727</v>
       </c>
-      <c r="B94" s="10" t="s">
+      <c r="B94" s="9" t="s">
         <v>697</v>
       </c>
-      <c r="C94" s="10" t="s">
+      <c r="C94" s="9" t="s">
         <v>592</v>
       </c>
     </row>
@@ -3728,10 +3720,10 @@
       <c r="A95" s="9" t="s">
         <v>717</v>
       </c>
-      <c r="B95" s="10" t="s">
+      <c r="B95" s="9" t="s">
         <v>688</v>
       </c>
-      <c r="C95" s="10" t="s">
+      <c r="C95" s="9" t="s">
         <v>594</v>
       </c>
     </row>
@@ -3739,10 +3731,10 @@
       <c r="A96" s="9" t="s">
         <v>718</v>
       </c>
-      <c r="B96" s="10" t="s">
+      <c r="B96" s="9" t="s">
         <v>694</v>
       </c>
-      <c r="C96" s="10" t="s">
+      <c r="C96" s="9" t="s">
         <v>596</v>
       </c>
     </row>
@@ -3750,164 +3742,164 @@
       <c r="A97" s="9" t="s">
         <v>719</v>
       </c>
-      <c r="B97" s="10" t="s">
+      <c r="B97" s="9" t="s">
         <v>695</v>
       </c>
-      <c r="C97" s="10" t="s">
+      <c r="C97" s="9" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="98" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A98" s="10" t="s">
+    <row r="98" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A98" s="9" t="s">
         <v>691</v>
       </c>
-      <c r="B98" s="10" t="s">
+      <c r="B98" s="9" t="s">
         <v>689</v>
       </c>
       <c r="C98" s="8" t="s">
         <v>573</v>
       </c>
     </row>
-    <row r="99" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A99" s="10" t="s">
+    <row r="99" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A99" s="9" t="s">
         <v>703</v>
       </c>
-      <c r="B99" s="10" t="s">
+      <c r="B99" s="9" t="s">
         <v>699</v>
       </c>
-      <c r="C99" s="10" t="s">
+      <c r="C99" s="9" t="s">
         <v>575</v>
       </c>
     </row>
-    <row r="100" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A100" s="10" t="s">
+    <row r="100" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A100" s="9" t="s">
         <v>704</v>
       </c>
-      <c r="B100" s="10" t="s">
+      <c r="B100" s="9" t="s">
         <v>690</v>
       </c>
       <c r="C100" s="8" t="s">
         <v>579</v>
       </c>
     </row>
-    <row r="101" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A101" s="10" t="s">
+    <row r="101" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A101" s="9" t="s">
         <v>705</v>
       </c>
-      <c r="B101" s="10" t="s">
+      <c r="B101" s="9" t="s">
         <v>700</v>
       </c>
       <c r="C101" s="8" t="s">
         <v>581</v>
       </c>
     </row>
-    <row r="102" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A102" s="10" t="s">
+    <row r="102" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A102" s="9" t="s">
         <v>706</v>
       </c>
-      <c r="B102" s="10" t="s">
+      <c r="B102" s="9" t="s">
         <v>702</v>
       </c>
       <c r="C102" s="8" t="s">
         <v>583</v>
       </c>
     </row>
-    <row r="103" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A103" s="10" t="s">
+    <row r="103" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A103" s="9" t="s">
         <v>707</v>
       </c>
-      <c r="B103" s="10" t="s">
+      <c r="B103" s="9" t="s">
         <v>701</v>
       </c>
       <c r="C103" s="8" t="s">
         <v>585</v>
       </c>
     </row>
-    <row r="104" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A104" s="10" t="s">
+    <row r="104" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A104" s="9" t="s">
         <v>708</v>
       </c>
-      <c r="B104" s="10" t="s">
+      <c r="B104" s="9" t="s">
         <v>696</v>
       </c>
       <c r="C104" s="8" t="s">
         <v>587</v>
       </c>
     </row>
-    <row r="105" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A105" s="10" t="s">
+    <row r="105" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A105" s="9" t="s">
         <v>709</v>
       </c>
-      <c r="B105" s="10" t="s">
+      <c r="B105" s="9" t="s">
         <v>714</v>
       </c>
-      <c r="C105" s="10" t="s">
+      <c r="C105" s="9" t="s">
         <v>715</v>
       </c>
     </row>
-    <row r="106" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A106" s="10" t="s">
+    <row r="106" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A106" s="9" t="s">
         <v>710</v>
       </c>
-      <c r="B106" s="10" t="s">
+      <c r="B106" s="9" t="s">
         <v>697</v>
       </c>
-      <c r="C106" s="10" t="s">
+      <c r="C106" s="9" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="107" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A107" s="10" t="s">
+    <row r="107" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A107" s="9" t="s">
         <v>692</v>
       </c>
-      <c r="B107" s="10" t="s">
+      <c r="B107" s="9" t="s">
         <v>688</v>
       </c>
-      <c r="C107" s="10" t="s">
+      <c r="C107" s="9" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="108" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A108" s="10" t="s">
+    <row r="108" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A108" s="9" t="s">
         <v>693</v>
       </c>
-      <c r="B108" s="10" t="s">
+      <c r="B108" s="9" t="s">
         <v>687</v>
       </c>
-      <c r="C108" s="10" t="s">
+      <c r="C108" s="9" t="s">
         <v>605</v>
       </c>
     </row>
-    <row r="109" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A109" s="10" t="s">
+    <row r="109" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A109" s="9" t="s">
         <v>711</v>
       </c>
-      <c r="B109" s="10" t="s">
+      <c r="B109" s="9" t="s">
         <v>694</v>
       </c>
-      <c r="C109" s="10" t="s">
+      <c r="C109" s="9" t="s">
         <v>596</v>
       </c>
     </row>
-    <row r="110" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A110" s="10" t="s">
+    <row r="110" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A110" s="9" t="s">
         <v>712</v>
       </c>
-      <c r="B110" s="10" t="s">
+      <c r="B110" s="9" t="s">
         <v>695</v>
       </c>
-      <c r="C110" s="10" t="s">
+      <c r="C110" s="9" t="s">
         <v>599</v>
       </c>
     </row>
-    <row r="111" spans="1:3" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A111" s="10" t="s">
+    <row r="111" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A111" s="9" t="s">
         <v>713</v>
       </c>
-      <c r="B111" s="10" t="s">
+      <c r="B111" s="9" t="s">
         <v>698</v>
       </c>
-      <c r="C111" s="10" t="s">
+      <c r="C111" s="9" t="s">
         <v>605</v>
       </c>
     </row>
@@ -4982,1004 +4974,1004 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:E58"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="B22" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="16.875" style="13" customWidth="1"/>
+    <col min="1" max="1" width="16.875" style="10" customWidth="1"/>
     <col min="2" max="2" width="10.875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="82.25" style="13" customWidth="1"/>
+    <col min="3" max="3" width="82.25" style="10" customWidth="1"/>
     <col min="4" max="4" width="84" style="6" customWidth="1"/>
-    <col min="5" max="5" width="25" style="13" customWidth="1"/>
-    <col min="6" max="1025" width="10.5" style="13" customWidth="1"/>
-    <col min="1026" max="16384" width="9" style="13"/>
+    <col min="5" max="5" width="25" style="10" customWidth="1"/>
+    <col min="6" max="1025" width="10.5" style="10" customWidth="1"/>
+    <col min="1026" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A1" s="13" t="s">
+      <c r="A1" s="10" t="s">
         <v>309</v>
       </c>
       <c r="B1" s="6" t="s">
         <v>310</v>
       </c>
-      <c r="C1" s="13" t="s">
+      <c r="C1" s="10" t="s">
         <v>311</v>
       </c>
       <c r="D1" s="6" t="s">
         <v>312</v>
       </c>
-      <c r="E1" s="13" t="s">
+      <c r="E1" s="10" t="s">
         <v>669</v>
       </c>
     </row>
     <row r="2" spans="1:5" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="13" t="s">
+      <c r="A2" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B2" s="6">
         <v>8.1</v>
       </c>
-      <c r="C2" s="13" t="s">
+      <c r="C2" s="10" t="s">
         <v>314</v>
       </c>
       <c r="D2" s="6" t="s">
         <v>315</v>
       </c>
-      <c r="E2" s="13" t="s">
+      <c r="E2" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="3" spans="1:5" ht="16.350000000000001" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="13" t="s">
+      <c r="A3" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B3" s="6">
         <v>8.1999999999999993</v>
       </c>
-      <c r="C3" s="13" t="s">
+      <c r="C3" s="10" t="s">
         <v>316</v>
       </c>
       <c r="D3" s="6" t="s">
         <v>317</v>
       </c>
-      <c r="E3" s="13" t="s">
+      <c r="E3" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A4" s="13" t="s">
+      <c r="A4" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B4" s="6">
         <v>8.3000000000000007</v>
       </c>
-      <c r="C4" s="13" t="s">
+      <c r="C4" s="10" t="s">
         <v>318</v>
       </c>
       <c r="D4" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="E4" s="13" t="s">
+      <c r="E4" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" s="13" t="s">
+      <c r="A5" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B5" s="6">
         <v>8.4</v>
       </c>
-      <c r="C5" s="13" t="s">
+      <c r="C5" s="10" t="s">
         <v>320</v>
       </c>
       <c r="D5" s="6" t="s">
         <v>321</v>
       </c>
-      <c r="E5" s="13" t="s">
+      <c r="E5" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A6" s="13" t="s">
+      <c r="A6" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B6" s="6">
         <v>8.5</v>
       </c>
-      <c r="C6" s="13" t="s">
+      <c r="C6" s="10" t="s">
         <v>322</v>
       </c>
       <c r="D6" s="6" t="s">
         <v>323</v>
       </c>
-      <c r="E6" s="13" t="s">
+      <c r="E6" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A7" s="13" t="s">
+      <c r="A7" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B7" s="6">
         <v>8.6</v>
       </c>
-      <c r="C7" s="13" t="s">
+      <c r="C7" s="10" t="s">
         <v>324</v>
       </c>
       <c r="D7" s="6" t="s">
         <v>325</v>
       </c>
-      <c r="E7" s="13" t="s">
+      <c r="E7" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A8" s="13" t="s">
+      <c r="A8" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B8" s="6">
         <v>8.6999999999999993</v>
       </c>
-      <c r="C8" s="13" t="s">
+      <c r="C8" s="10" t="s">
         <v>326</v>
       </c>
       <c r="D8" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="E8" s="13" t="s">
+      <c r="E8" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A9" s="13" t="s">
+      <c r="A9" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B9" s="6">
         <v>8.8000000000000007</v>
       </c>
-      <c r="C9" s="13" t="s">
+      <c r="C9" s="10" t="s">
         <v>327</v>
       </c>
       <c r="D9" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="E9" s="13" t="s">
+      <c r="E9" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A10" s="13" t="s">
+      <c r="A10" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B10" s="6">
         <v>8.9</v>
       </c>
-      <c r="C10" s="13" t="s">
+      <c r="C10" s="10" t="s">
         <v>328</v>
       </c>
       <c r="D10" s="6" t="s">
         <v>319</v>
       </c>
-      <c r="E10" s="13" t="s">
+      <c r="E10" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A11" s="13" t="s">
+      <c r="A11" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>329</v>
       </c>
-      <c r="C11" s="13" t="s">
+      <c r="C11" s="10" t="s">
         <v>330</v>
       </c>
       <c r="D11" s="6" t="s">
         <v>331</v>
       </c>
-      <c r="E11" s="13" t="s">
+      <c r="E11" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A12" s="13" t="s">
+      <c r="A12" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>332</v>
       </c>
-      <c r="C12" s="13" t="s">
+      <c r="C12" s="10" t="s">
         <v>745</v>
       </c>
       <c r="D12" s="6" t="s">
         <v>333</v>
       </c>
-      <c r="E12" s="13" t="s">
+      <c r="E12" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A13" s="13" t="s">
+      <c r="A13" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>334</v>
       </c>
-      <c r="C13" s="13" t="s">
+      <c r="C13" s="10" t="s">
         <v>746</v>
       </c>
       <c r="D13" s="6">
         <v>76.5</v>
       </c>
-      <c r="E13" s="13" t="s">
+      <c r="E13" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>335</v>
       </c>
-      <c r="C14" s="13" t="s">
+      <c r="C14" s="10" t="s">
         <v>744</v>
       </c>
       <c r="D14" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="E14" s="13" t="s">
+      <c r="E14" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="15" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="13" t="s">
+      <c r="A15" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>337</v>
       </c>
-      <c r="C15" s="13" t="s">
+      <c r="C15" s="10" t="s">
         <v>743</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="E15" s="13" t="s">
+      <c r="E15" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="16" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="13" t="s">
+      <c r="A16" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>339</v>
       </c>
-      <c r="C16" s="12" t="s">
+      <c r="C16" s="6" t="s">
         <v>748</v>
       </c>
       <c r="D16" s="8" t="s">
         <v>728</v>
       </c>
-      <c r="E16" s="13" t="s">
+      <c r="E16" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="17" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="13" t="s">
+      <c r="A17" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B17" s="6" t="s">
         <v>340</v>
       </c>
-      <c r="C17" s="12" t="s">
+      <c r="C17" s="6" t="s">
         <v>761</v>
       </c>
       <c r="D17" s="8" t="s">
         <v>729</v>
       </c>
-      <c r="E17" s="13" t="s">
+      <c r="E17" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A18" s="13" t="s">
+      <c r="A18" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B18" s="6" t="s">
         <v>341</v>
       </c>
-      <c r="C18" s="12" t="s">
+      <c r="C18" s="6" t="s">
         <v>747</v>
       </c>
       <c r="D18" s="8" t="s">
         <v>730</v>
       </c>
-      <c r="E18" s="13" t="s">
+      <c r="E18" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B19" s="6" t="s">
         <v>342</v>
       </c>
-      <c r="C19" s="12" t="s">
+      <c r="C19" s="6" t="s">
         <v>760</v>
       </c>
       <c r="D19" s="8" t="s">
         <v>731</v>
       </c>
-      <c r="E19" s="13" t="s">
+      <c r="E19" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="20" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A20" s="13" t="s">
+      <c r="A20" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B20" s="6" t="s">
         <v>343</v>
       </c>
-      <c r="C20" s="12" t="s">
+      <c r="C20" s="6" t="s">
         <v>749</v>
       </c>
       <c r="D20" s="8" t="s">
         <v>732</v>
       </c>
-      <c r="E20" s="13" t="s">
+      <c r="E20" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A21" s="13" t="s">
+      <c r="A21" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B21" s="6" t="s">
         <v>344</v>
       </c>
-      <c r="C21" s="12" t="s">
+      <c r="C21" s="6" t="s">
         <v>742</v>
       </c>
       <c r="D21" s="8" t="s">
         <v>733</v>
       </c>
-      <c r="E21" s="13" t="s">
+      <c r="E21" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="22" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="13" t="s">
+      <c r="A22" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B22" s="6" t="s">
         <v>345</v>
       </c>
-      <c r="C22" s="12" t="s">
+      <c r="C22" s="6" t="s">
         <v>752</v>
       </c>
       <c r="D22" s="8" t="s">
         <v>734</v>
       </c>
-      <c r="E22" s="13" t="s">
+      <c r="E22" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="23" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="13" t="s">
+      <c r="A23" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B23" s="6" t="s">
         <v>346</v>
       </c>
-      <c r="C23" s="12" t="s">
+      <c r="C23" s="6" t="s">
         <v>751</v>
       </c>
       <c r="D23" s="8" t="s">
         <v>735</v>
       </c>
-      <c r="E23" s="13" t="s">
+      <c r="E23" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A24" s="13" t="s">
+      <c r="A24" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B24" s="6" t="s">
         <v>347</v>
       </c>
-      <c r="C24" s="12" t="s">
+      <c r="C24" s="6" t="s">
         <v>753</v>
       </c>
       <c r="D24" s="8" t="s">
         <v>736</v>
       </c>
-      <c r="E24" s="13" t="s">
+      <c r="E24" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="25" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="13" t="s">
+      <c r="A25" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B25" s="6" t="s">
         <v>348</v>
       </c>
-      <c r="C25" s="13" t="s">
+      <c r="C25" s="10" t="s">
         <v>762</v>
       </c>
       <c r="D25" s="6" t="s">
         <v>349</v>
       </c>
-      <c r="E25" s="13" t="s">
+      <c r="E25" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="26" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="13" t="s">
+      <c r="A26" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B26" s="6" t="s">
         <v>350</v>
       </c>
-      <c r="C26" s="13" t="s">
+      <c r="C26" s="10" t="s">
         <v>763</v>
       </c>
       <c r="D26" s="6" t="s">
         <v>351</v>
       </c>
-      <c r="E26" s="13" t="s">
+      <c r="E26" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A27" s="13" t="s">
+      <c r="A27" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B27" s="6" t="s">
         <v>352</v>
       </c>
-      <c r="C27" s="13" t="s">
+      <c r="C27" s="10" t="s">
         <v>764</v>
       </c>
       <c r="D27" s="6" t="s">
         <v>336</v>
       </c>
-      <c r="E27" s="13" t="s">
+      <c r="E27" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="28" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="13" t="s">
+      <c r="A28" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B28" s="6" t="s">
         <v>353</v>
       </c>
-      <c r="C28" s="13" t="s">
+      <c r="C28" s="10" t="s">
         <v>765</v>
       </c>
       <c r="D28" s="6" t="s">
         <v>338</v>
       </c>
-      <c r="E28" s="13" t="s">
+      <c r="E28" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A29" s="13" t="s">
+      <c r="A29" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B29" s="6" t="s">
         <v>354</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="10" t="s">
         <v>766</v>
       </c>
       <c r="D29" s="8" t="s">
         <v>728</v>
       </c>
-      <c r="E29" s="13" t="s">
+      <c r="E29" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="30" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="13" t="s">
+      <c r="A30" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B30" s="6" t="s">
         <v>355</v>
       </c>
-      <c r="C30" s="13" t="s">
+      <c r="C30" s="10" t="s">
         <v>767</v>
       </c>
       <c r="D30" s="8" t="s">
         <v>729</v>
       </c>
-      <c r="E30" s="13" t="s">
+      <c r="E30" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A31" s="13" t="s">
+      <c r="A31" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B31" s="6" t="s">
         <v>356</v>
       </c>
-      <c r="C31" s="13" t="s">
+      <c r="C31" s="10" t="s">
         <v>768</v>
       </c>
       <c r="D31" s="8" t="s">
         <v>730</v>
       </c>
-      <c r="E31" s="13" t="s">
+      <c r="E31" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A32" s="13" t="s">
+      <c r="A32" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B32" s="6" t="s">
         <v>357</v>
       </c>
-      <c r="C32" s="13" t="s">
+      <c r="C32" s="10" t="s">
         <v>769</v>
       </c>
       <c r="D32" s="8" t="s">
         <v>731</v>
       </c>
-      <c r="E32" s="13" t="s">
+      <c r="E32" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="33" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A33" s="13" t="s">
+      <c r="A33" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B33" s="6" t="s">
         <v>358</v>
       </c>
-      <c r="C33" s="13" t="s">
+      <c r="C33" s="10" t="s">
         <v>770</v>
       </c>
       <c r="D33" s="8" t="s">
         <v>732</v>
       </c>
-      <c r="E33" s="13" t="s">
+      <c r="E33" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A34" s="13" t="s">
+      <c r="A34" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B34" s="6" t="s">
         <v>359</v>
       </c>
-      <c r="C34" s="13" t="s">
+      <c r="C34" s="10" t="s">
         <v>772</v>
       </c>
       <c r="D34" s="8" t="s">
         <v>733</v>
       </c>
-      <c r="E34" s="13" t="s">
+      <c r="E34" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="35" spans="1:5" ht="47.25" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B35" s="6" t="s">
         <v>360</v>
       </c>
-      <c r="C35" s="13" t="s">
+      <c r="C35" s="10" t="s">
         <v>771</v>
       </c>
       <c r="D35" s="8" t="s">
         <v>734</v>
       </c>
-      <c r="E35" s="13" t="s">
+      <c r="E35" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="36" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A36" s="13" t="s">
+      <c r="A36" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B36" s="6" t="s">
         <v>361</v>
       </c>
-      <c r="C36" s="13" t="s">
+      <c r="C36" s="10" t="s">
         <v>774</v>
       </c>
       <c r="D36" s="8" t="s">
         <v>735</v>
       </c>
-      <c r="E36" s="13" t="s">
+      <c r="E36" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A37" s="13" t="s">
+      <c r="A37" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B37" s="6" t="s">
         <v>362</v>
       </c>
-      <c r="C37" s="13" t="s">
+      <c r="C37" s="10" t="s">
         <v>773</v>
       </c>
       <c r="D37" s="8" t="s">
         <v>736</v>
       </c>
-      <c r="E37" s="13" t="s">
+      <c r="E37" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="38" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A38" s="13" t="s">
+      <c r="A38" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B38" s="6" t="s">
         <v>363</v>
       </c>
-      <c r="C38" s="13" t="s">
+      <c r="C38" s="10" t="s">
         <v>364</v>
       </c>
       <c r="D38" s="6" t="s">
         <v>365</v>
       </c>
-      <c r="E38" s="13" t="s">
+      <c r="E38" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="39" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A39" s="13" t="s">
+      <c r="A39" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B39" s="6" t="s">
         <v>366</v>
       </c>
-      <c r="C39" s="13" t="s">
+      <c r="C39" s="10" t="s">
         <v>367</v>
       </c>
       <c r="D39" s="6" t="s">
         <v>368</v>
       </c>
-      <c r="E39" s="13" t="s">
+      <c r="E39" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="40" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A40" s="13" t="s">
+      <c r="A40" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B40" s="6" t="s">
         <v>369</v>
       </c>
-      <c r="C40" s="13" t="s">
+      <c r="C40" s="10" t="s">
         <v>370</v>
       </c>
       <c r="D40" s="6" t="s">
         <v>371</v>
       </c>
-      <c r="E40" s="13" t="s">
+      <c r="E40" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="41" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A41" s="13" t="s">
+      <c r="A41" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B41" s="6" t="s">
         <v>372</v>
       </c>
-      <c r="C41" s="13" t="s">
+      <c r="C41" s="10" t="s">
         <v>373</v>
       </c>
       <c r="D41" s="6" t="s">
         <v>374</v>
       </c>
-      <c r="E41" s="13" t="s">
+      <c r="E41" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A42" s="13" t="s">
+      <c r="A42" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B42" s="6" t="s">
         <v>375</v>
       </c>
-      <c r="C42" s="13" t="s">
+      <c r="C42" s="10" t="s">
         <v>376</v>
       </c>
       <c r="D42" s="6" t="s">
         <v>377</v>
       </c>
-      <c r="E42" s="13" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A43" s="13" t="s">
+      <c r="E42" s="10" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="43" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A43" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B43" s="6" t="s">
         <v>378</v>
       </c>
-      <c r="C43" s="13" t="s">
+      <c r="C43" s="10" t="s">
         <v>379</v>
       </c>
       <c r="D43" s="6" t="s">
         <v>380</v>
       </c>
-      <c r="E43" s="13" t="s">
+      <c r="E43" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A44" s="13" t="s">
+      <c r="A44" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B44" s="6" t="s">
         <v>381</v>
       </c>
-      <c r="C44" s="13" t="s">
+      <c r="C44" s="10" t="s">
         <v>382</v>
       </c>
       <c r="D44" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="E44" s="13" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A45" s="13" t="s">
+      <c r="E44" s="10" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A45" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B45" s="6" t="s">
         <v>384</v>
       </c>
-      <c r="C45" s="13" t="s">
+      <c r="C45" s="10" t="s">
         <v>385</v>
       </c>
       <c r="D45" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="E45" s="13" t="s">
+      <c r="E45" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A46" s="13" t="s">
+      <c r="A46" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B46" s="6" t="s">
         <v>387</v>
       </c>
-      <c r="C46" s="13" t="s">
+      <c r="C46" s="10" t="s">
         <v>388</v>
       </c>
       <c r="D46" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="E46" s="13" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A47" s="13" t="s">
+      <c r="E46" s="10" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A47" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B47" s="6" t="s">
         <v>389</v>
       </c>
-      <c r="C47" s="13" t="s">
+      <c r="C47" s="10" t="s">
         <v>390</v>
       </c>
       <c r="D47" s="6" t="s">
         <v>386</v>
       </c>
-      <c r="E47" s="13" t="s">
+      <c r="E47" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A48" s="13" t="s">
+      <c r="A48" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B48" s="6" t="s">
         <v>391</v>
       </c>
-      <c r="C48" s="13" t="s">
+      <c r="C48" s="10" t="s">
         <v>392</v>
       </c>
       <c r="D48" s="6" t="s">
         <v>383</v>
       </c>
-      <c r="E48" s="13" t="s">
+      <c r="E48" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="49" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
-      <c r="A49" s="13" t="s">
+      <c r="A49" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B49" s="6" t="s">
         <v>393</v>
       </c>
-      <c r="C49" s="13" t="s">
+      <c r="C49" s="10" t="s">
         <v>394</v>
       </c>
       <c r="D49" s="6" t="s">
         <v>395</v>
       </c>
-      <c r="E49" s="13" t="s">
+      <c r="E49" s="10" t="s">
         <v>668</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A50" s="13" t="s">
+      <c r="A50" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B50" s="6" t="s">
         <v>396</v>
       </c>
-      <c r="C50" s="13" t="s">
+      <c r="C50" s="10" t="s">
         <v>397</v>
       </c>
       <c r="D50" s="6" t="s">
         <v>398</v>
       </c>
-      <c r="E50" s="13" t="s">
+      <c r="E50" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B51" s="6" t="s">
         <v>399</v>
       </c>
-      <c r="C51" s="13" t="s">
+      <c r="C51" s="10" t="s">
         <v>400</v>
       </c>
       <c r="D51" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="E51" s="13" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A52" s="13" t="s">
+      <c r="E51" s="10" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="52" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A52" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B52" s="6" t="s">
         <v>402</v>
       </c>
-      <c r="C52" s="13" t="s">
+      <c r="C52" s="10" t="s">
         <v>403</v>
       </c>
       <c r="D52" s="6" t="s">
         <v>404</v>
       </c>
-      <c r="E52" s="13" t="s">
+      <c r="E52" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A53" s="13" t="s">
+      <c r="A53" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B53" s="6" t="s">
         <v>405</v>
       </c>
-      <c r="C53" s="13" t="s">
+      <c r="C53" s="10" t="s">
         <v>406</v>
       </c>
       <c r="D53" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="E53" s="13" t="s">
+      <c r="E53" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A54" s="13" t="s">
+      <c r="A54" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B54" s="6" t="s">
         <v>407</v>
       </c>
-      <c r="C54" s="13" t="s">
+      <c r="C54" s="10" t="s">
         <v>408</v>
       </c>
       <c r="D54" s="6" t="s">
         <v>409</v>
       </c>
-      <c r="E54" s="13" t="s">
+      <c r="E54" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A55" s="13" t="s">
+      <c r="A55" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B55" s="6" t="s">
         <v>410</v>
       </c>
-      <c r="C55" s="13" t="s">
+      <c r="C55" s="10" t="s">
         <v>411</v>
       </c>
       <c r="D55" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="E55" s="13" t="s">
+      <c r="E55" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A56" s="13" t="s">
+      <c r="A56" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B56" s="6" t="s">
         <v>412</v>
       </c>
-      <c r="C56" s="13" t="s">
+      <c r="C56" s="10" t="s">
         <v>413</v>
       </c>
       <c r="D56" s="6" t="s">
         <v>414</v>
       </c>
-      <c r="E56" s="13" t="s">
+      <c r="E56" s="10" t="s">
         <v>665</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A57" s="13" t="s">
+      <c r="A57" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B57" s="6" t="s">
         <v>415</v>
       </c>
-      <c r="C57" s="13" t="s">
+      <c r="C57" s="10" t="s">
         <v>416</v>
       </c>
       <c r="D57" s="6" t="s">
         <v>401</v>
       </c>
-      <c r="E57" s="13" t="s">
-        <v>665</v>
-      </c>
-    </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A58" s="13" t="s">
+      <c r="E57" s="10" t="s">
+        <v>665</v>
+      </c>
+    </row>
+    <row r="58" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="10" t="s">
         <v>313</v>
       </c>
       <c r="B58" s="6" t="s">
         <v>417</v>
       </c>
-      <c r="C58" s="13" t="s">
+      <c r="C58" s="10" t="s">
         <v>418</v>
       </c>
       <c r="D58" s="6" t="s">
         <v>419</v>
       </c>
-      <c r="E58" s="13" t="s">
+      <c r="E58" s="10" t="s">
         <v>665</v>
       </c>
     </row>
@@ -6611,17 +6603,17 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:E51"/>
+  <dimension ref="A1:D51"/>
   <sheetViews>
-    <sheetView topLeftCell="A28" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B42" sqref="B42"/>
+    <sheetView tabSelected="1" topLeftCell="A34" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C39" sqref="C39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="10.875" style="6" customWidth="1"/>
-    <col min="2" max="2" width="80.875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="31.125" style="6" customWidth="1"/>
+    <col min="2" max="2" width="42" style="6" customWidth="1"/>
+    <col min="3" max="3" width="69.125" style="6" customWidth="1"/>
     <col min="4" max="1026" width="10.5" style="6" customWidth="1"/>
     <col min="1027" max="16384" width="9" style="6"/>
   </cols>
@@ -6908,7 +6900,7 @@
       <c r="B26" s="6" t="s">
         <v>548</v>
       </c>
-      <c r="D26" s="14" t="s">
+      <c r="D26" s="11" t="s">
         <v>667</v>
       </c>
     </row>
@@ -6978,7 +6970,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A33" s="6" t="s">
         <v>561</v>
       </c>
@@ -6989,7 +6981,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A34" s="6" t="s">
         <v>563</v>
       </c>
@@ -7000,7 +6992,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A35" s="6" t="s">
         <v>565</v>
       </c>
@@ -7011,7 +7003,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A36" s="6" t="s">
         <v>567</v>
       </c>
@@ -7022,7 +7014,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A37" s="6" t="s">
         <v>569</v>
       </c>
@@ -7033,7 +7025,7 @@
         <v>665</v>
       </c>
     </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A38" s="6" t="s">
         <v>571</v>
       </c>
@@ -7044,57 +7036,51 @@
         <v>665</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>728</v>
       </c>
       <c r="B39" s="8" t="s">
-        <v>777</v>
+        <v>775</v>
       </c>
       <c r="C39" s="8" t="s">
-        <v>775</v>
+        <v>782</v>
       </c>
       <c r="D39" s="8"/>
-      <c r="E39" s="6" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="40" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="40" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>729</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>778</v>
+        <v>776</v>
       </c>
       <c r="C40" s="8"/>
       <c r="D40" s="8"/>
     </row>
-    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>730</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>779</v>
+        <v>777</v>
       </c>
       <c r="C41" s="8"/>
       <c r="D41" s="8"/>
     </row>
-    <row r="42" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>731</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>780</v>
+        <v>778</v>
       </c>
       <c r="C42" s="8" t="s">
-        <v>785</v>
+        <v>783</v>
       </c>
       <c r="D42" s="8"/>
-      <c r="E42" s="6" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="43" spans="1:5" ht="78.75" x14ac:dyDescent="0.25">
+    </row>
+    <row r="43" spans="1:4" ht="78.75" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>732</v>
       </c>
@@ -7102,48 +7088,45 @@
         <v>754</v>
       </c>
       <c r="C43" s="8" t="s">
-        <v>776</v>
+        <v>784</v>
       </c>
       <c r="D43" s="8"/>
-      <c r="E43" s="6" t="s">
-        <v>784</v>
-      </c>
-    </row>
-    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
+    </row>
+    <row r="44" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>733</v>
       </c>
       <c r="B44" s="8" t="s">
-        <v>781</v>
+        <v>779</v>
       </c>
       <c r="C44" s="8" t="s">
         <v>750</v>
       </c>
       <c r="D44" s="8"/>
     </row>
-    <row r="45" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>734</v>
       </c>
       <c r="B45" s="8" t="s">
-        <v>782</v>
+        <v>780</v>
       </c>
       <c r="C45" s="8"/>
       <c r="D45" s="8"/>
     </row>
-    <row r="46" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>735</v>
       </c>
       <c r="B46" s="8" t="s">
-        <v>783</v>
+        <v>781</v>
       </c>
       <c r="C46" s="8"/>
-      <c r="D46" s="15" t="s">
+      <c r="D46" s="12" t="s">
         <v>737</v>
       </c>
     </row>
-    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>736</v>
       </c>
@@ -7153,7 +7136,7 @@
       <c r="C47" s="8"/>
       <c r="D47" s="8"/>
     </row>
-    <row r="48" spans="1:5" ht="31.5" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:4" ht="31.5" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>738</v>
       </c>
@@ -7205,7 +7188,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:E24"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A10" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>

</xml_diff>